<commit_message>
Finalized filter of H observations at IPTDS for scenario 1.
</commit_message>
<xml_diff>
--- a/data/PIT_Tag_R-Group.xlsx
+++ b/data/PIT_Tag_R-Group.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\LGR_pHOS_Sim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F2E4A2-39C5-4634-A766-3B7D9FCECDD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Release Data" sheetId="1" r:id="rId1"/>
@@ -18,10 +19,16 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Release Data'!$A$1:$K$144</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -276,7 +283,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -359,11 +366,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -645,69 +652,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2018</v>
       </c>
@@ -746,7 +753,7 @@
         <v>67.202472435683262</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2018</v>
       </c>
@@ -785,7 +792,7 @@
         <v>60.252747252747255</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2018</v>
       </c>
@@ -824,7 +831,7 @@
         <v>70.05236198064884</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2018</v>
       </c>
@@ -863,7 +870,7 @@
         <v>57.577961939840392</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2018</v>
       </c>
@@ -902,7 +909,7 @@
         <v>86.126566673515512</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2018</v>
       </c>
@@ -941,7 +948,7 @@
         <v>111.05885790616129</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2018</v>
       </c>
@@ -981,7 +988,7 @@
         <v>103.82981418918919</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2018</v>
       </c>
@@ -1020,7 +1027,7 @@
         <v>104.74347942995429</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2018</v>
       </c>
@@ -1059,7 +1066,7 @@
         <v>75.040732221583283</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2018</v>
       </c>
@@ -1098,7 +1105,7 @@
         <v>4.8787120453787116</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2018</v>
       </c>
@@ -1137,7 +1144,7 @@
         <v>123.14295125164691</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2018</v>
       </c>
@@ -1176,7 +1183,7 @@
         <v>142.05049180327867</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2018</v>
       </c>
@@ -1215,7 +1222,7 @@
         <v>28.320811570912014</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2018</v>
       </c>
@@ -1254,7 +1261,7 @@
         <v>35.139698492462308</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2018</v>
       </c>
@@ -1293,7 +1300,7 @@
         <v>70.577930333079081</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2018</v>
       </c>
@@ -1332,7 +1339,7 @@
         <v>67.235990660440294</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2018</v>
       </c>
@@ -1371,7 +1378,7 @@
         <v>63.77183872938302</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2018</v>
       </c>
@@ -1410,7 +1417,7 @@
         <v>93.821795519622711</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2018</v>
       </c>
@@ -1449,7 +1456,7 @@
         <v>127.33685800604229</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2018</v>
       </c>
@@ -1488,7 +1495,7 @@
         <v>109.20533498759305</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2018</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>128.92233166478283</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>2017</v>
       </c>
@@ -1571,7 +1578,7 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>2017</v>
       </c>
@@ -1610,7 +1617,7 @@
         <v>71.802813599062134</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2017</v>
       </c>
@@ -1649,7 +1656,7 @@
         <v>72.7</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2017</v>
       </c>
@@ -1688,7 +1695,7 @@
         <v>71.040000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2017</v>
       </c>
@@ -1727,7 +1734,7 @@
         <v>101.88</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2017</v>
       </c>
@@ -1766,7 +1773,7 @@
         <v>110.52</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2017</v>
       </c>
@@ -1805,7 +1812,7 @@
         <v>97.72</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2017</v>
       </c>
@@ -1844,7 +1851,7 @@
         <v>100.75</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2017</v>
       </c>
@@ -1883,7 +1890,7 @@
         <v>69.319999999999993</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2017</v>
       </c>
@@ -1922,7 +1929,7 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2017</v>
       </c>
@@ -1961,7 +1968,7 @@
         <v>265.94</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2017</v>
       </c>
@@ -2000,7 +2007,7 @@
         <v>30.91</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2017</v>
       </c>
@@ -2039,7 +2046,7 @@
         <v>31.77</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2017</v>
       </c>
@@ -2078,7 +2085,7 @@
         <v>69.510000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>2017</v>
       </c>
@@ -2117,7 +2124,7 @@
         <v>49.354086256083235</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2017</v>
       </c>
@@ -2156,7 +2163,7 @@
         <v>44.03</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2017</v>
       </c>
@@ -2195,7 +2202,7 @@
         <v>92.67</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2017</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>133.85</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2017</v>
       </c>
@@ -2273,7 +2280,7 @@
         <v>129.11000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2017</v>
       </c>
@@ -2312,7 +2319,7 @@
         <v>127.55</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2016</v>
       </c>
@@ -2351,7 +2358,7 @@
         <v>81.319758192809417</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2016</v>
       </c>
@@ -2390,7 +2397,7 @@
         <v>77.318244170096023</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2016</v>
       </c>
@@ -2429,7 +2436,7 @@
         <v>34.208392942298524</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2016</v>
       </c>
@@ -2468,7 +2475,7 @@
         <v>70.507138607971442</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2016</v>
       </c>
@@ -2507,7 +2514,7 @@
         <v>104.42618675013041</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2016</v>
       </c>
@@ -2546,7 +2553,7 @@
         <v>104.04046486421389</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2016</v>
       </c>
@@ -2585,7 +2592,7 @@
         <v>108.65195702225633</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2016</v>
       </c>
@@ -2624,7 +2631,7 @@
         <v>83.128451047788005</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2016</v>
       </c>
@@ -2663,7 +2670,7 @@
         <v>10.03271913208197</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2016</v>
       </c>
@@ -2702,7 +2709,7 @@
         <v>124.77036048064086</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2016</v>
       </c>
@@ -2741,7 +2748,7 @@
         <v>142.98025016458197</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2016</v>
       </c>
@@ -2780,7 +2787,7 @@
         <v>70.924981055822172</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2016</v>
       </c>
@@ -2819,7 +2826,7 @@
         <v>31.158749492488834</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2016</v>
       </c>
@@ -2858,7 +2865,7 @@
         <v>31.459302325581394</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2016</v>
       </c>
@@ -2897,7 +2904,7 @@
         <v>67.351446246447082</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2016</v>
       </c>
@@ -2936,7 +2943,7 @@
         <v>68.026732981038236</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2016</v>
       </c>
@@ -2975,7 +2982,7 @@
         <v>70.841741534208708</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2016</v>
       </c>
@@ -3014,7 +3021,7 @@
         <v>99.650437514022883</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2016</v>
       </c>
@@ -3053,7 +3060,7 @@
         <v>127.71793587174349</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2016</v>
       </c>
@@ -3092,7 +3099,7 @@
         <v>131.8890266584005</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2016</v>
       </c>
@@ -3131,7 +3138,7 @@
         <v>129.5164463076427</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2015</v>
       </c>
@@ -3170,7 +3177,7 @@
         <v>63.57</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2015</v>
       </c>
@@ -3209,7 +3216,7 @@
         <v>81.38</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2015</v>
       </c>
@@ -3248,7 +3255,7 @@
         <v>29.31</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2015</v>
       </c>
@@ -3287,7 +3294,7 @@
         <v>68.56</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2015</v>
       </c>
@@ -3326,7 +3333,7 @@
         <v>159.37</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2015</v>
       </c>
@@ -3365,7 +3372,7 @@
         <v>100.1</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2015</v>
       </c>
@@ -3404,7 +3411,7 @@
         <v>98.73</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2015</v>
       </c>
@@ -3443,7 +3450,7 @@
         <v>81.099999999999994</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2015</v>
       </c>
@@ -3473,7 +3480,7 @@
         <v>123785</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2015</v>
       </c>
@@ -3512,7 +3519,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2015</v>
       </c>
@@ -3551,7 +3558,7 @@
         <v>13.14</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2015</v>
       </c>
@@ -3590,7 +3597,7 @@
         <v>84.06</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2015</v>
       </c>
@@ -3629,7 +3636,7 @@
         <v>113.88</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2015</v>
       </c>
@@ -3668,7 +3675,7 @@
         <v>130.46</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>2015</v>
       </c>
@@ -3707,7 +3714,7 @@
         <v>142.4</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>2015</v>
       </c>
@@ -3746,7 +3753,7 @@
         <v>30.41</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>2015</v>
       </c>
@@ -3785,7 +3792,7 @@
         <v>31.71</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>2015</v>
       </c>
@@ -3824,7 +3831,7 @@
         <v>68.180000000000007</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>2015</v>
       </c>
@@ -3863,7 +3870,7 @@
         <v>70.48</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>2015</v>
       </c>
@@ -3902,7 +3909,7 @@
         <v>95.9</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>2015</v>
       </c>
@@ -3941,7 +3948,7 @@
         <v>40.19</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>2015</v>
       </c>
@@ -3980,7 +3987,7 @@
         <v>59.96</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>2015</v>
       </c>
@@ -4019,7 +4026,7 @@
         <v>56.52</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>2015</v>
       </c>
@@ -4049,7 +4056,7 @@
         <v>55970</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>2015</v>
       </c>
@@ -4088,7 +4095,7 @@
         <v>94.68</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>2015</v>
       </c>
@@ -4127,7 +4134,7 @@
         <v>136.33000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>2015</v>
       </c>
@@ -4166,7 +4173,7 @@
         <v>125.34</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>2015</v>
       </c>
@@ -4205,7 +4212,7 @@
         <v>133.16999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>2014</v>
       </c>
@@ -4244,7 +4251,7 @@
         <v>86.503348214285722</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>2014</v>
       </c>
@@ -4283,7 +4290,7 @@
         <v>124.33406352683463</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>2014</v>
       </c>
@@ -4322,7 +4329,7 @@
         <v>47.127910586774291</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>2014</v>
       </c>
@@ -4361,7 +4368,7 @@
         <v>42.07431442327821</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>2014</v>
       </c>
@@ -4400,7 +4407,7 @@
         <v>145.61393596986818</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>2014</v>
       </c>
@@ -4439,7 +4446,7 @@
         <v>123.09020902090209</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>2014</v>
       </c>
@@ -4478,7 +4485,7 @@
         <v>55.635164835164836</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>2014</v>
       </c>
@@ -4517,7 +4524,7 @@
         <v>109.8013778156204</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>2014</v>
       </c>
@@ -4556,7 +4563,7 @@
         <v>112.5931899641577</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>2014</v>
       </c>
@@ -4595,7 +4602,7 @@
         <v>79.257142857142867</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>2014</v>
       </c>
@@ -4625,7 +4632,7 @@
         <v>128381</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>2014</v>
       </c>
@@ -4664,7 +4671,7 @@
         <v>73.411541423698978</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>2014</v>
       </c>
@@ -4703,7 +4710,7 @@
         <v>9.8391900937081669</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>2014</v>
       </c>
@@ -4742,7 +4749,7 @@
         <v>142.5929003021148</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>2014</v>
       </c>
@@ -4781,7 +4788,7 @@
         <v>239.58189929891654</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>2014</v>
       </c>
@@ -4820,7 +4827,7 @@
         <v>21.700394218134033</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>2014</v>
       </c>
@@ -4859,7 +4866,7 @@
         <v>23.428137651821864</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>2014</v>
       </c>
@@ -4898,7 +4905,7 @@
         <v>23.161684105630293</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>2014</v>
       </c>
@@ -4937,7 +4944,7 @@
         <v>120.77692307692307</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>2014</v>
       </c>
@@ -4976,7 +4983,7 @@
         <v>115.30498533724341</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>2014</v>
       </c>
@@ -5015,7 +5022,7 @@
         <v>51.538400633412508</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>2014</v>
       </c>
@@ -5054,7 +5061,7 @@
         <v>51.335702341137129</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>2014</v>
       </c>
@@ -5093,7 +5100,7 @@
         <v>49.977497039084085</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>2014</v>
       </c>
@@ -5132,7 +5139,7 @@
         <v>51.513077171456253</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>2014</v>
       </c>
@@ -5171,7 +5178,7 @@
         <v>96.593553859202714</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>2014</v>
       </c>
@@ -5210,7 +5217,7 @@
         <v>117.32156862745099</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>2014</v>
       </c>
@@ -5249,7 +5256,7 @@
         <v>144.69792251544075</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>2014</v>
       </c>
@@ -5288,7 +5295,7 @@
         <v>131.88689234718433</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>2013</v>
       </c>
@@ -5327,7 +5334,7 @@
         <v>77.180089485458609</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>2013</v>
       </c>
@@ -5366,7 +5373,7 @@
         <v>178.21052631578945</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>2013</v>
       </c>
@@ -5405,7 +5412,7 @@
         <v>37.452178267401102</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>2013</v>
       </c>
@@ -5444,7 +5451,7 @@
         <v>26.531759979914639</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>2013</v>
       </c>
@@ -5483,7 +5490,7 @@
         <v>126.45514636449481</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>2013</v>
       </c>
@@ -5522,7 +5529,7 @@
         <v>123.68860619469027</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>2013</v>
       </c>
@@ -5561,7 +5568,7 @@
         <v>332.31881371640407</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>2013</v>
       </c>
@@ -5600,7 +5607,7 @@
         <v>102.01593931128538</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>2013</v>
       </c>
@@ -5639,7 +5646,7 @@
         <v>45.5953531598513</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>2013</v>
       </c>
@@ -5678,7 +5685,7 @@
         <v>124.74251497005987</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>2013</v>
       </c>
@@ -5708,7 +5715,7 @@
         <v>118874</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>2013</v>
       </c>
@@ -5747,7 +5754,7 @@
         <v>211.14304857621443</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>2013</v>
       </c>
@@ -5786,7 +5793,7 @@
         <v>9.588494077834179</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>2013</v>
       </c>
@@ -5825,7 +5832,7 @@
         <v>73.798418972332016</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>2013</v>
       </c>
@@ -5864,7 +5871,7 @@
         <v>128.25275437459496</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>2013</v>
       </c>
@@ -5903,7 +5910,7 @@
         <v>154.41639557579703</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>2013</v>
       </c>
@@ -5942,7 +5949,7 @@
         <v>16.820983033932137</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>2013</v>
       </c>
@@ -5981,7 +5988,7 @@
         <v>69.07726269315674</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>2013</v>
       </c>
@@ -6020,7 +6027,7 @@
         <v>69.90902255639098</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>2013</v>
       </c>
@@ -6059,7 +6066,7 @@
         <v>138.24498886414256</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>2013</v>
       </c>
@@ -6098,7 +6105,7 @@
         <v>64.898193760262728</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>2013</v>
       </c>
@@ -6137,7 +6144,7 @@
         <v>63.602470522178542</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>2013</v>
       </c>
@@ -6176,7 +6183,7 @@
         <v>97.105414066453037</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>2013</v>
       </c>
@@ -6215,7 +6222,7 @@
         <v>125.78397711015737</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>2013</v>
       </c>
@@ -6261,50 +6268,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4:O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:15" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="4" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="4" spans="2:15" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>